<commit_message>
in picks excel added forumas to check if pick is correct
</commit_message>
<xml_diff>
--- a/Predictions_1-26-23.xlsx
+++ b/Predictions_1-26-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\261378\Desktop\ProgrammingPractice\PythonPractice\CBB_Score_Predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1E99DEB-F518-412D-B77F-DE098BCB42ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042E1921-ABBA-4BA7-9994-8C3285D08E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-16425" windowWidth="29040" windowHeight="15840" xr2:uid="{7DEDD8E8-3F3D-4278-8009-32DEE7B3E2BD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Home</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Arizona State</t>
+  </si>
+  <si>
+    <t>Winning Team</t>
   </si>
 </sst>
 </file>
@@ -194,7 +197,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -212,9 +221,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6D250323-617B-4CFC-84A2-30353679C8C3}" name="Table2" displayName="Table2" ref="A1:E27" totalsRowShown="0">
-  <autoFilter ref="A1:E27" xr:uid="{6D250323-617B-4CFC-84A2-30353679C8C3}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6D250323-617B-4CFC-84A2-30353679C8C3}" name="Table2" displayName="Table2" ref="A1:F17" totalsRowShown="0">
+  <autoFilter ref="A1:F17" xr:uid="{6D250323-617B-4CFC-84A2-30353679C8C3}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{E57E3A88-EA27-4838-AF8F-A1200AF82B2B}" name="Home"/>
     <tableColumn id="2" xr3:uid="{12E078FB-6DF2-4850-A31E-2A7AEB7C471B}" name="Away"/>
     <tableColumn id="3" xr3:uid="{219EC8DF-F23F-4424-94B7-703202740116}" name="Home Score"/>
@@ -222,19 +231,25 @@
     <tableColumn id="5" xr3:uid="{0EE8292D-F8A3-4E48-BF9B-7ADF17803C8C}" name="Margin">
       <calculatedColumnFormula>C2-D2</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="6" xr3:uid="{94CF7CC5-F5A5-4338-81D4-F7D9667A8582}" name="Winning Team" dataDxfId="1">
+      <calculatedColumnFormula>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B798BF99-0713-425B-AD04-ACB598A718E7}" name="Table3" displayName="Table3" ref="G1:I27" totalsRowShown="0">
-  <autoFilter ref="G1:I27" xr:uid="{B798BF99-0713-425B-AD04-ACB598A718E7}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B798BF99-0713-425B-AD04-ACB598A718E7}" name="Table3" displayName="Table3" ref="H1:K17" totalsRowShown="0">
+  <autoFilter ref="H1:K17" xr:uid="{B798BF99-0713-425B-AD04-ACB598A718E7}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1401157E-E543-4183-BD5E-969FDB474A39}" name="Actual Home Score"/>
     <tableColumn id="2" xr3:uid="{7F0F381E-D158-43AF-B416-B01A705B5BFA}" name="Actual Away Score"/>
-    <tableColumn id="3" xr3:uid="{7F03D607-5FB8-47D2-8A50-61204329B714}" name="Actual Margin" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{7F03D607-5FB8-47D2-8A50-61204329B714}" name="Actual Margin" dataDxfId="2">
       <calculatedColumnFormula>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{745CCC7E-7195-4C37-B278-C548C309D894}" name="Winning Team" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -538,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F97BD59-2171-466B-8FD1-32C94A4B0A76}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,12 +565,14 @@
     <col min="2" max="2" width="11.6328125" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="12.54296875" customWidth="1"/>
-    <col min="7" max="7" width="18.7265625" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" customWidth="1"/>
+    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="9" max="9" width="9.90625" customWidth="1"/>
+    <col min="11" max="11" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -571,17 +588,23 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -598,12 +621,24 @@
         <f>C2-D2</f>
         <v>3</v>
       </c>
-      <c r="I2">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F2" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Home Wins</v>
+      </c>
+      <c r="J2">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K2" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M2" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Inccorect</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -620,12 +655,24 @@
         <f t="shared" ref="E3:E27" si="0">C3-D3</f>
         <v>-4</v>
       </c>
-      <c r="I3">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F3" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="J3">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K3" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M3" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -642,12 +689,24 @@
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
-      <c r="I4">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F4" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="J4">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K4" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M4" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -664,12 +723,24 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="I5">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F5" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Home Wins</v>
+      </c>
+      <c r="J5">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K5" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M5" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Inccorect</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -686,12 +757,24 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I6">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F6" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Home Wins</v>
+      </c>
+      <c r="J6">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K6" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M6" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Inccorect</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -708,12 +791,24 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="I7">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F7" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Home Wins</v>
+      </c>
+      <c r="J7">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K7" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M7" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Inccorect</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -730,12 +825,24 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="I8">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F8" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="J8">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K8" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M8" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -752,12 +859,24 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="I9">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F9" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Home Wins</v>
+      </c>
+      <c r="J9">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K9" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M9" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Inccorect</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -774,12 +893,24 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="I10">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F10" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Home Wins</v>
+      </c>
+      <c r="J10">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K10" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M10" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Inccorect</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -796,12 +927,24 @@
         <f t="shared" si="0"/>
         <v>-20</v>
       </c>
-      <c r="I11">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F11" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="J11">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K11" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M11" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -818,12 +961,24 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I12">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F12" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Home Wins</v>
+      </c>
+      <c r="J12">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K12" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M12" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Inccorect</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -840,12 +995,24 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="I13">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F13" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Home Wins</v>
+      </c>
+      <c r="J13">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K13" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M13" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Inccorect</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -862,12 +1029,24 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I14">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F14" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Home Wins</v>
+      </c>
+      <c r="J14">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K14" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M14" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Inccorect</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -884,12 +1063,24 @@
         <f t="shared" si="0"/>
         <v>-3</v>
       </c>
-      <c r="I15">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F15" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="J15">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K15" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M15" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Correct</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -906,12 +1097,24 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I16">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F16" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Home Wins</v>
+      </c>
+      <c r="J16">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K16" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M16" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Inccorect</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -928,116 +1131,29 @@
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
-      <c r="I17">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I25">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
-        <v>0</v>
+      <c r="F17" t="str">
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="J17">
+        <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
+        <v>0</v>
+      </c>
+      <c r="K17" t="str">
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
+        <v>Away Wins</v>
+      </c>
+      <c r="M17" t="str">
+        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <v>Correct</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added check for if team name isnt found
</commit_message>
<xml_diff>
--- a/Predictions_1-26-23.xlsx
+++ b/Predictions_1-26-23.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\261378\Desktop\ProgrammingPractice\PythonPractice\CBB_Score_Predictor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042E1921-ABBA-4BA7-9994-8C3285D08E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD41CC87-6602-465F-9414-6408BDA3F368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-16425" windowWidth="29040" windowHeight="15840" xr2:uid="{7DEDD8E8-3F3D-4278-8009-32DEE7B3E2BD}"/>
   </bookViews>
@@ -155,7 +155,7 @@
     <t>Arizona State</t>
   </si>
   <si>
-    <t>Winning Team</t>
+    <t>Home Result</t>
   </si>
 </sst>
 </file>
@@ -231,8 +231,8 @@
     <tableColumn id="5" xr3:uid="{0EE8292D-F8A3-4E48-BF9B-7ADF17803C8C}" name="Margin">
       <calculatedColumnFormula>C2-D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{94CF7CC5-F5A5-4338-81D4-F7D9667A8582}" name="Winning Team" dataDxfId="1">
-      <calculatedColumnFormula>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{94CF7CC5-F5A5-4338-81D4-F7D9667A8582}" name="Home Result" dataDxfId="1">
+      <calculatedColumnFormula>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -248,8 +248,8 @@
     <tableColumn id="3" xr3:uid="{7F03D607-5FB8-47D2-8A50-61204329B714}" name="Actual Margin" dataDxfId="2">
       <calculatedColumnFormula>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{745CCC7E-7195-4C37-B278-C548C309D894}" name="Winning Team" dataDxfId="0">
-      <calculatedColumnFormula>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{745CCC7E-7195-4C37-B278-C548C309D894}" name="Home Result" dataDxfId="0">
+      <calculatedColumnFormula>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -556,7 +556,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -622,19 +622,19 @@
         <v>3</v>
       </c>
       <c r="F2" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Home Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>W</v>
       </c>
       <c r="J2">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K2" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M2" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Inccorect</v>
       </c>
     </row>
@@ -652,23 +652,23 @@
         <v>76</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E27" si="0">C3-D3</f>
+        <f t="shared" ref="E3:E17" si="0">C3-D3</f>
         <v>-4</v>
       </c>
       <c r="F3" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>L</v>
       </c>
       <c r="J3">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K3" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M3" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Correct</v>
       </c>
     </row>
@@ -690,19 +690,19 @@
         <v>-4</v>
       </c>
       <c r="F4" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>L</v>
       </c>
       <c r="J4">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K4" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M4" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Correct</v>
       </c>
     </row>
@@ -724,19 +724,19 @@
         <v>17</v>
       </c>
       <c r="F5" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Home Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>W</v>
       </c>
       <c r="J5">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K5" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M5" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Inccorect</v>
       </c>
     </row>
@@ -758,19 +758,19 @@
         <v>6</v>
       </c>
       <c r="F6" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Home Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>W</v>
       </c>
       <c r="J6">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K6" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M6" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Inccorect</v>
       </c>
     </row>
@@ -792,19 +792,19 @@
         <v>18</v>
       </c>
       <c r="F7" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Home Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>W</v>
       </c>
       <c r="J7">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K7" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M7" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Inccorect</v>
       </c>
     </row>
@@ -826,19 +826,19 @@
         <v>-2</v>
       </c>
       <c r="F8" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>L</v>
       </c>
       <c r="J8">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K8" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M8" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Correct</v>
       </c>
     </row>
@@ -860,19 +860,19 @@
         <v>23</v>
       </c>
       <c r="F9" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Home Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>W</v>
       </c>
       <c r="J9">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K9" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M9" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Inccorect</v>
       </c>
     </row>
@@ -894,19 +894,19 @@
         <v>44</v>
       </c>
       <c r="F10" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Home Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>W</v>
       </c>
       <c r="J10">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K10" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M10" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Inccorect</v>
       </c>
     </row>
@@ -928,19 +928,19 @@
         <v>-20</v>
       </c>
       <c r="F11" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>L</v>
       </c>
       <c r="J11">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K11" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M11" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Correct</v>
       </c>
     </row>
@@ -962,19 +962,19 @@
         <v>2</v>
       </c>
       <c r="F12" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Home Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>W</v>
       </c>
       <c r="J12">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K12" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M12" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Inccorect</v>
       </c>
     </row>
@@ -996,19 +996,19 @@
         <v>21</v>
       </c>
       <c r="F13" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Home Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>W</v>
       </c>
       <c r="J13">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K13" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M13" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Inccorect</v>
       </c>
     </row>
@@ -1030,19 +1030,19 @@
         <v>10</v>
       </c>
       <c r="F14" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Home Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>W</v>
       </c>
       <c r="J14">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K14" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M14" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Inccorect</v>
       </c>
     </row>
@@ -1064,19 +1064,19 @@
         <v>-3</v>
       </c>
       <c r="F15" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>L</v>
       </c>
       <c r="J15">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K15" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M15" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Correct</v>
       </c>
     </row>
@@ -1098,19 +1098,19 @@
         <v>4</v>
       </c>
       <c r="F16" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Home Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>W</v>
       </c>
       <c r="J16">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K16" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M16" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Inccorect</v>
       </c>
     </row>
@@ -1132,19 +1132,19 @@
         <v>-2</v>
       </c>
       <c r="F17" t="str">
-        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table2[[#This Row],[Home Score]]&gt;Table2[[#This Row],[Away Score]],"W", "L")</f>
+        <v>L</v>
       </c>
       <c r="J17">
         <f>Table3[[#This Row],[Actual Home Score]]-Table3[[#This Row],[Actual Away Score]]</f>
         <v>0</v>
       </c>
       <c r="K17" t="str">
-        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "Home Wins", "Away Wins")</f>
-        <v>Away Wins</v>
+        <f>IF(Table3[[#This Row],[Actual Home Score]]&gt;Table3[[#This Row],[Actual Away Score]], "W", "L")</f>
+        <v>L</v>
       </c>
       <c r="M17" t="str">
-        <f>+IF(Table2[[#This Row],[Winning Team]]=Table3[[#This Row],[Winning Team]], "Correct", "Inccorect")</f>
+        <f>+IF(Table2[[#This Row],[Home Result]]=Table3[[#This Row],[Home Result]], "Correct", "Inccorect")</f>
         <v>Correct</v>
       </c>
     </row>

</xml_diff>